<commit_message>
RESTORE_END v0.3 - Added passenger cars (fossil) - Plotting improvements
</commit_message>
<xml_diff>
--- a/data/interim_calc/passenger_private_cars.xlsx
+++ b/data/interim_calc/passenger_private_cars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/interim_calc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C9CC13-F537-D541-AC12-DBCF3A3E5BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531DEC55-8CBD-BA41-8C7C-92EDC40A2285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" xr2:uid="{E49C977C-9B4E-8A48-BAF4-9B3D30D216BD}"/>
+    <workbookView xWindow="38400" yWindow="13120" windowWidth="21600" windowHeight="19900" xr2:uid="{E49C977C-9B4E-8A48-BAF4-9B3D30D216BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
     <t>activity (Mvkt)</t>
   </si>
   <si>
-    <t>average Mvkm/unit</t>
+    <t>average hourly Mvkm/unit</t>
   </si>
 </sst>
 </file>
@@ -686,10 +686,10 @@
   <dimension ref="A1:BE36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AP8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BB35" sqref="BB35"/>
+      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -701,6 +701,7 @@
     <col min="46" max="46" width="13" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="48" max="52" width="12.1640625" customWidth="1"/>
+    <col min="54" max="54" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6414,8 +6415,8 @@
     </row>
     <row r="35" spans="13:57" x14ac:dyDescent="0.2">
       <c r="BB35">
-        <f>AVERAGE(BB3:BB32)</f>
-        <v>1.2886736514116322E-2</v>
+        <f>AVERAGE(BB3:BB32)/8760</f>
+        <v>1.4710886431639637E-6</v>
       </c>
       <c r="BE35">
         <f>AVERAGE(BE3:BE32)</f>
@@ -6427,36 +6428,36 @@
         <v>27</v>
       </c>
       <c r="N36">
-        <f>MAX(N3:N32)</f>
-        <v>314281</v>
+        <f>ROUND(MAX(N3:N32)*1.1,0)</f>
+        <v>345709</v>
       </c>
       <c r="O36">
-        <f t="shared" ref="O36:U36" si="41">MAX(O3:O32)</f>
-        <v>18285</v>
+        <f t="shared" ref="O36:U36" si="41">ROUND(MAX(O3:O32)*1.1,0)</f>
+        <v>20114</v>
       </c>
       <c r="P36">
         <f t="shared" si="41"/>
-        <v>4199</v>
+        <v>4619</v>
       </c>
       <c r="Q36">
         <f t="shared" si="41"/>
-        <v>127899</v>
+        <v>140689</v>
       </c>
       <c r="R36">
         <f t="shared" si="41"/>
-        <v>3847</v>
+        <v>4232</v>
       </c>
       <c r="S36">
         <f t="shared" si="41"/>
-        <v>281</v>
+        <v>309</v>
       </c>
       <c r="T36">
         <f t="shared" si="41"/>
-        <v>13177</v>
+        <v>14495</v>
       </c>
       <c r="U36">
         <f t="shared" si="41"/>
-        <v>1653</v>
+        <v>1818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>